<commit_message>
modular auto navigation added. user input allows to navigate to any screen required. excel reader made efficient to handle user inputs.
</commit_message>
<xml_diff>
--- a/resources/Parameters.xlsx
+++ b/resources/Parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-474960" yWindow="-480555" windowWidth="13095" windowHeight="5760"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17010" windowHeight="4785"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -33,9 +34,6 @@
     <t>param4</t>
   </si>
   <si>
-    <t>TC_Pclass_NV_NA_dsDNA_parameters</t>
-  </si>
-  <si>
     <t>Volume</t>
   </si>
   <si>
@@ -69,31 +67,34 @@
     <t>miRNA Sequence</t>
   </si>
   <si>
-    <t>TC_Pclass_NV_NA_ssDNA_parameters</t>
-  </si>
-  <si>
-    <t>TC_Pclass_NV_NA_RNA_parameters</t>
-  </si>
-  <si>
-    <t>TC_Pclass_NV_NA_miRNA_parameters</t>
-  </si>
-  <si>
-    <t>TC_Pclass_NV_NA_miRNASequence_parameters</t>
-  </si>
-  <si>
-    <t>TC_Pclass_NV_NA_Oligo_parameters</t>
-  </si>
-  <si>
-    <t>TC_Pclass_NV_NA_OligoSequence_parameters</t>
-  </si>
-  <si>
-    <t>TC_Pclass_NV_NA_NucleicAcid_parameters</t>
-  </si>
-  <si>
     <t>Nucleic Acid</t>
   </si>
   <si>
     <t>Volume222</t>
+  </si>
+  <si>
+    <t>TC_P-Class_Nucleic Acid_dsDNA_parameters</t>
+  </si>
+  <si>
+    <t>TC_P-Class_Nucleic Acid_ssDNA_parameters</t>
+  </si>
+  <si>
+    <t>TC_P-Class_Nucleic Acid_RNA_parameters</t>
+  </si>
+  <si>
+    <t>TC_P-Class_Nucleic Acid_miRNA_parameters</t>
+  </si>
+  <si>
+    <t>TC_P-Class_Nucleic Acid_miRNASequence_parameters</t>
+  </si>
+  <si>
+    <t>TC_P-Class_Nucleic Acid_Oligo_parameters</t>
+  </si>
+  <si>
+    <t>TC_P-Class_Nucleic Acid_OligoSequence_parameters</t>
+  </si>
+  <si>
+    <t>TC_P-Class_Nucleic Acid_NucleicAcid_parameters</t>
   </si>
 </sst>
 </file>
@@ -440,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,184 +475,185 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>